<commit_message>
regenerated exports after BOM change
</commit_message>
<xml_diff>
--- a/HW/PCB_TOP/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_TOP(Alarm Clock).xlsx
+++ b/HW/PCB_TOP/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_TOP(Alarm Clock).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7470F446-4C3A-4381-9E28-D49CE8EAAF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D02AB73-C210-473B-ABE4-EF62C8244920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{BA310D90-FD2D-4A59-990F-B020F17F07DF}"/>
+    <workbookView xWindow="5115" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{421F60A7-A67A-40AC-983C-A249FB7DE48C}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Timer_Clock_TOP(Al" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="147">
   <si>
     <t>Quantity</t>
   </si>
@@ -396,6 +396,27 @@
     <t>C104939</t>
   </si>
   <si>
+    <t>R518, R519, R520</t>
+  </si>
+  <si>
+    <t>R 270k 0402</t>
+  </si>
+  <si>
+    <t>RES 270K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>RC0402FR-07270KL</t>
+  </si>
+  <si>
+    <t>R_270k_0402</t>
+  </si>
+  <si>
+    <t>311-270KLRCT-ND</t>
+  </si>
+  <si>
     <t>R500, R501, R503, R504</t>
   </si>
   <si>
@@ -405,9 +426,6 @@
     <t>RES 10K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
@@ -417,6 +435,24 @@
     <t>311-10.0KLRCT-ND</t>
   </si>
   <si>
+    <t>R511, R512, R514, R515</t>
+  </si>
+  <si>
+    <t>R 16k 0402</t>
+  </si>
+  <si>
+    <t>RES 16K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RMCF0402FT16K0</t>
+  </si>
+  <si>
+    <t>R_16k_0402</t>
+  </si>
+  <si>
+    <t>RMCF0402FT16K0CT-ND</t>
+  </si>
+  <si>
     <t>R505, R507, R508, R516, R517</t>
   </si>
   <si>
@@ -433,24 +469,6 @@
   </si>
   <si>
     <t>RMCF0402ZT0R00CT-ND</t>
-  </si>
-  <si>
-    <t>R511, R512, R514, R515, R518, R519, R520</t>
-  </si>
-  <si>
-    <t>R 16k 0402</t>
-  </si>
-  <si>
-    <t>RES 16K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RMCF0402FT16K0</t>
-  </si>
-  <si>
-    <t>R_16k_0402</t>
-  </si>
-  <si>
-    <t>RMCF0402FT16K0CT-ND</t>
   </si>
 </sst>
 </file>
@@ -833,8 +851,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F16870-99BE-4620-A724-46712A74FE69}">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D6F3AA-1191-4DD6-8027-90AB1FA4A23E}">
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1364,7 +1382,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>122</v>
@@ -1396,7 +1414,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>129</v>
@@ -1411,7 +1429,7 @@
         <v>131</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>132</v>
@@ -1428,7 +1446,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>135</v>
@@ -1456,6 +1474,38 @@
       </c>
       <c r="J19" s="3" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>